<commit_message>
stacking fix in input sheet
</commit_message>
<xml_diff>
--- a/apps/fcft/Facility Sankey Tool - Input Sheet.xlsx
+++ b/apps/fcft/Facility Sankey Tool - Input Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/ovkhan_ucdavis_edu/Documents/git/ucdavis-shinyr/apps/fcft/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/ovkhan_ucdavis_edu/Documents/git/IAC-Decarb-Tools/apps/fcft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{7A74CD4C-D93B-4C6B-A887-33DE3185116F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6918202B-15B7-4EDF-8972-E22D1E543DAA}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{7A74CD4C-D93B-4C6B-A887-33DE3185116F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{031A5AF8-C59F-47F1-9538-9F7E3DAFD49F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="686" activeTab="3" xr2:uid="{ECAE08BA-56FE-4434-8B68-666D0954C98F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="686" activeTab="3" xr2:uid="{ECAE08BA-56FE-4434-8B68-666D0954C98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="12" r:id="rId1"/>
@@ -219,7 +219,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3041,7 +3041,7 @@
   <dimension ref="A1:Y792"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18528,8 +18528,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B1:T793"/>
   <sheetViews>
-    <sheetView topLeftCell="G6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6:T6"/>
+    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22558,7 +22558,7 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{285D5B68-F8D9-4B0C-ADC3-9324B819503F}">
           <x14:formula1>
             <xm:f>'Grid Emissions Database - AER'!$C$3:$L$3</xm:f>
@@ -22588,7 +22588,7 @@
   <dimension ref="A2:AF792"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22714,14 +22714,18 @@
       <c r="B7" s="61" t="str" cm="1">
         <f t="array" ref="B7:B18">_xlfn.VSTACK(
     _xlfn._xlws.FILTER('Energy Inputs'!B7:B189, 'Energy Inputs'!B7:B189 &lt;&gt; ""),
-    _xlfn._xlws.FILTER('Emission Inputs (Optional)'!G9:G191, 'Emission Inputs (Optional)'!G9:G191 &lt;&gt; "")
+    IF(COUNTA('Emission Inputs (Optional)'!G9:G191) &gt; 0,
+        _xlfn._xlws.FILTER('Emission Inputs (Optional)'!G9:G191, 'Emission Inputs (Optional)'!G9:G191 &lt;&gt; ""),
+        "")
 )</f>
         <v>HVAC-Electrical</v>
       </c>
-      <c r="C7" s="70" t="str" cm="1">
+      <c r="C7" s="61" t="str" cm="1">
         <f t="array" ref="C7:C18">_xlfn.VSTACK(
     _xlfn._xlws.FILTER('Energy Inputs'!C7:C189, 'Energy Inputs'!C7:C189 &lt;&gt; ""),
-    _xlfn._xlws.FILTER('Emission Inputs (Optional)'!H9:H191, 'Emission Inputs (Optional)'!H9:H191 &lt;&gt; "")
+    IF(COUNTA('Emission Inputs (Optional)'!H9:H191) &gt; 0,
+        _xlfn._xlws.FILTER('Emission Inputs (Optional)'!H9:H191, 'Emission Inputs (Optional)'!H9:H191 &lt;&gt; ""),
+        "")
 )</f>
         <v>Energy</v>
       </c>
@@ -48999,7 +49003,7 @@
   <dimension ref="B1:O57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C1" sqref="C1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Input Sheet Fix (#6)
* stacking fix in input sheet

* lc input sheet fix
</commit_message>
<xml_diff>
--- a/apps/fcft/Facility Sankey Tool - Input Sheet.xlsx
+++ b/apps/fcft/Facility Sankey Tool - Input Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/ovkhan_ucdavis_edu/Documents/git/ucdavis-shinyr/apps/fcft/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/ovkhan_ucdavis_edu/Documents/git/IAC-Decarb-Tools/apps/fcft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{7A74CD4C-D93B-4C6B-A887-33DE3185116F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6918202B-15B7-4EDF-8972-E22D1E543DAA}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{7A74CD4C-D93B-4C6B-A887-33DE3185116F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{031A5AF8-C59F-47F1-9538-9F7E3DAFD49F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="686" activeTab="3" xr2:uid="{ECAE08BA-56FE-4434-8B68-666D0954C98F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="686" activeTab="3" xr2:uid="{ECAE08BA-56FE-4434-8B68-666D0954C98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="12" r:id="rId1"/>
@@ -219,7 +219,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3041,7 +3041,7 @@
   <dimension ref="A1:Y792"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18528,8 +18528,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B1:T793"/>
   <sheetViews>
-    <sheetView topLeftCell="G6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6:T6"/>
+    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22558,7 +22558,7 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{285D5B68-F8D9-4B0C-ADC3-9324B819503F}">
           <x14:formula1>
             <xm:f>'Grid Emissions Database - AER'!$C$3:$L$3</xm:f>
@@ -22588,7 +22588,7 @@
   <dimension ref="A2:AF792"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22714,14 +22714,18 @@
       <c r="B7" s="61" t="str" cm="1">
         <f t="array" ref="B7:B18">_xlfn.VSTACK(
     _xlfn._xlws.FILTER('Energy Inputs'!B7:B189, 'Energy Inputs'!B7:B189 &lt;&gt; ""),
-    _xlfn._xlws.FILTER('Emission Inputs (Optional)'!G9:G191, 'Emission Inputs (Optional)'!G9:G191 &lt;&gt; "")
+    IF(COUNTA('Emission Inputs (Optional)'!G9:G191) &gt; 0,
+        _xlfn._xlws.FILTER('Emission Inputs (Optional)'!G9:G191, 'Emission Inputs (Optional)'!G9:G191 &lt;&gt; ""),
+        "")
 )</f>
         <v>HVAC-Electrical</v>
       </c>
-      <c r="C7" s="70" t="str" cm="1">
+      <c r="C7" s="61" t="str" cm="1">
         <f t="array" ref="C7:C18">_xlfn.VSTACK(
     _xlfn._xlws.FILTER('Energy Inputs'!C7:C189, 'Energy Inputs'!C7:C189 &lt;&gt; ""),
-    _xlfn._xlws.FILTER('Emission Inputs (Optional)'!H9:H191, 'Emission Inputs (Optional)'!H9:H191 &lt;&gt; "")
+    IF(COUNTA('Emission Inputs (Optional)'!H9:H191) &gt; 0,
+        _xlfn._xlws.FILTER('Emission Inputs (Optional)'!H9:H191, 'Emission Inputs (Optional)'!H9:H191 &lt;&gt; ""),
+        "")
 )</f>
         <v>Energy</v>
       </c>
@@ -48999,7 +49003,7 @@
   <dimension ref="B1:O57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C1" sqref="C1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>